<commit_message>
updated conversion between kW and PJ
</commit_message>
<xml_diff>
--- a/references/offline-calculations/levelized_cost_of_energy.xlsx
+++ b/references/offline-calculations/levelized_cost_of_energy.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/alexanderkell/Documents/SGI/Projects/11-starter-kits/references/offline-calculations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{484A754D-590B-6F42-BE5D-904FBCFC3193}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5F302A1D-042C-294F-B15E-7705D8F60437}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="500" windowWidth="28800" windowHeight="17500" xr2:uid="{63C303C4-630A-5A43-A01D-43786B1DCA90}"/>
   </bookViews>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="25">
   <si>
     <t xml:space="preserve">LCOE = </t>
   </si>
@@ -45,21 +45,6 @@
     <t>((Investment costs + O&amp;M costs + Fuel costs)/(1+discount rate)) / (Electrical Energy Produced in year t/ (1+discount rate))</t>
   </si>
   <si>
-    <t>Column3</t>
-  </si>
-  <si>
-    <t>Column4</t>
-  </si>
-  <si>
-    <t>Column5</t>
-  </si>
-  <si>
-    <t>Column6</t>
-  </si>
-  <si>
-    <t>Column7</t>
-  </si>
-  <si>
     <t>Technology</t>
   </si>
   <si>
@@ -67,12 +52,72 @@
   </si>
   <si>
     <t>Coal power plant</t>
+  </si>
+  <si>
+    <t>cap_par</t>
+  </si>
+  <si>
+    <t>fix_par</t>
+  </si>
+  <si>
+    <t>Lifetime</t>
+  </si>
+  <si>
+    <t>Utilization Factor</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>LCOE</t>
+  </si>
+  <si>
+    <t>capacity</t>
+  </si>
+  <si>
+    <t>Capital costs</t>
+  </si>
+  <si>
+    <t>Production</t>
+  </si>
+  <si>
+    <t>Onshore wind</t>
+  </si>
+  <si>
+    <t>Fixed costs</t>
+  </si>
+  <si>
+    <t>Interest rate</t>
+  </si>
+  <si>
+    <t>Fuel Cost Rate (MUSD/PJ)</t>
+  </si>
+  <si>
+    <t>Discounted rate</t>
+  </si>
+  <si>
+    <t>Sum</t>
+  </si>
+  <si>
+    <t>Discounted number</t>
+  </si>
+  <si>
+    <t>Fuel Costs</t>
+  </si>
+  <si>
+    <t>HEAT RATE = COMM_IN VALUE</t>
+  </si>
+  <si>
+    <t>CommIn</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="171" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -108,13 +153,41 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="171" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="8">
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="1" formatCode="0"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="0" formatCode="General"/>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -128,16 +201,54 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D083B2D7-23A2-3B43-BAE9-D1CECE76F5C0}" name="Table1" displayName="Table1" ref="A5:G28" totalsRowShown="0">
-  <autoFilter ref="A5:G28" xr:uid="{D083B2D7-23A2-3B43-BAE9-D1CECE76F5C0}"/>
-  <tableColumns count="7">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{D083B2D7-23A2-3B43-BAE9-D1CECE76F5C0}" name="Table1" displayName="Table1" ref="A5:Q28" totalsRowShown="0">
+  <autoFilter ref="A5:Q28" xr:uid="{D083B2D7-23A2-3B43-BAE9-D1CECE76F5C0}"/>
+  <tableColumns count="17">
     <tableColumn id="1" xr3:uid="{B88D60DD-C215-D644-9154-C5188A912713}" name="Technology"/>
     <tableColumn id="2" xr3:uid="{6F26CD7E-C5CC-4A4B-9450-1654FD656CC7}" name="Year"/>
-    <tableColumn id="3" xr3:uid="{04666FE0-1967-0946-8FA8-C26FD8C5D314}" name="Column3"/>
-    <tableColumn id="4" xr3:uid="{42346E1A-2343-D042-9853-EBAE1621BF7D}" name="Column4"/>
-    <tableColumn id="5" xr3:uid="{F30EA145-3649-944B-9402-72B3D8309DEF}" name="Column5"/>
-    <tableColumn id="6" xr3:uid="{10A77899-D5FA-E348-9257-56AAB8315F68}" name="Column6"/>
-    <tableColumn id="7" xr3:uid="{5EE6C10E-B7A4-814E-BD44-40B9359BDFDF}" name="Column7"/>
+    <tableColumn id="17" xr3:uid="{15411392-953F-5348-AA4D-8EEF17E3CF6C}" name="CommIn"/>
+    <tableColumn id="14" xr3:uid="{C9273737-823C-FF4A-9801-2A74D02E8E7A}" name="Interest rate"/>
+    <tableColumn id="10" xr3:uid="{F49EA88A-433F-AB41-AAFB-0215F1407888}" name="capacity"/>
+    <tableColumn id="3" xr3:uid="{04666FE0-1967-0946-8FA8-C26FD8C5D314}" name="cap_par"/>
+    <tableColumn id="11" xr3:uid="{6AAE8B8E-1055-1B48-AF76-D1D0FAFB369F}" name="Capital costs" dataDxfId="1">
+      <calculatedColumnFormula>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="4" xr3:uid="{42346E1A-2343-D042-9853-EBAE1621BF7D}" name="fix_par"/>
+    <tableColumn id="12" xr3:uid="{E0EDE4EB-5264-6043-BAC9-D4D6A86010FF}" name="Fixed costs" dataDxfId="2">
+      <calculatedColumnFormula>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="5" xr3:uid="{F30EA145-3649-944B-9402-72B3D8309DEF}" name="Lifetime"/>
+    <tableColumn id="6" xr3:uid="{10A77899-D5FA-E348-9257-56AAB8315F68}" name="Utilization Factor"/>
+    <tableColumn id="13" xr3:uid="{F7548241-C7CA-7E47-A66F-5039D906E989}" name="Production" dataDxfId="6">
+      <calculatedColumnFormula>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="7" xr3:uid="{5EE6C10E-B7A4-814E-BD44-40B9359BDFDF}" name="Efficiency"/>
+    <tableColumn id="8" xr3:uid="{1EC84C3C-2A2D-B54C-A066-6B332E9F37D6}" name="Fuel Cost Rate (MUSD/PJ)"/>
+    <tableColumn id="15" xr3:uid="{89511566-9CB1-3F42-922A-98556A1D7613}" name="Fuel Costs" dataDxfId="0">
+      <calculatedColumnFormula>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="16" xr3:uid="{05FC7CC5-82AB-0040-9A24-548B513E2CFA}" name="Discounted number" dataDxfId="4">
+      <calculatedColumnFormula>VLOOKUP(J6,Table2[#All],3,FALSE)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="9" xr3:uid="{CA76B1B8-4C1D-1845-8771-197518E843B6}" name="LCOE" dataDxfId="3">
+      <calculatedColumnFormula>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</calculatedColumnFormula>
+    </tableColumn>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{AF73CAC1-3778-DE40-96B1-C2F24C75D2EB}" name="Table2" displayName="Table2" ref="U4:W39" totalsRowShown="0">
+  <autoFilter ref="U4:W39" xr:uid="{AF73CAC1-3778-DE40-96B1-C2F24C75D2EB}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{56C8394D-B5DA-834E-A70A-02A4DD3BC819}" name="Year"/>
+    <tableColumn id="2" xr3:uid="{11D9D777-BC8A-EA45-8FD8-5A74726B64D3}" name="Discounted rate" dataDxfId="7">
+      <calculatedColumnFormula>(1+$D$7)^Table2[[#This Row],[Year]]</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{3C6E0536-ED5B-294B-B069-89F461696DB7}" name="Sum" dataDxfId="5">
+      <calculatedColumnFormula>SUM($V$4:Table2[[#This Row],[Discounted rate]])</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -440,18 +551,29 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FE2663E8-969B-3546-9F10-324BEF8EE937}">
-  <dimension ref="A1:G6"/>
+  <dimension ref="A1:W39"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18.83203125" customWidth="1"/>
+    <col min="2" max="3" width="8.33203125" customWidth="1"/>
+    <col min="4" max="4" width="13.83203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="11.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.6640625" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="12.33203125" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="21" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="21" customWidth="1"/>
+    <col min="17" max="17" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="17.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -459,47 +581,1375 @@
         <v>1</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>0</v>
       </c>
       <c r="B2" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="M2" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="U4" t="s">
+        <v>4</v>
+      </c>
+      <c r="V4" t="s">
+        <v>19</v>
+      </c>
+      <c r="W4" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="D5" t="s">
-        <v>4</v>
+        <v>17</v>
       </c>
       <c r="E5" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="F5" t="s">
         <v>6</v>
       </c>
       <c r="G5" t="s">
+        <v>13</v>
+      </c>
+      <c r="H5" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="I5" t="s">
+        <v>16</v>
+      </c>
+      <c r="J5" t="s">
+        <v>8</v>
+      </c>
+      <c r="K5" t="s">
+        <v>9</v>
+      </c>
+      <c r="L5" t="s">
+        <v>14</v>
+      </c>
+      <c r="M5" t="s">
+        <v>10</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" t="s">
+        <v>22</v>
+      </c>
+      <c r="P5" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>11</v>
+      </c>
+      <c r="U5">
+        <v>1</v>
+      </c>
+      <c r="V5">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="W5">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>1.1000000000000001</v>
+      </c>
+    </row>
+    <row r="6" spans="1:23" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
+        <v>5</v>
+      </c>
+      <c r="B6">
+        <v>2050</v>
+      </c>
+      <c r="C6">
+        <v>2.7</v>
+      </c>
+      <c r="D6">
+        <v>0.1</v>
+      </c>
+      <c r="E6">
+        <v>10000</v>
+      </c>
+      <c r="F6" s="1">
+        <v>80.749354005167902</v>
+      </c>
+      <c r="G6" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>807493.54005167901</v>
+      </c>
+      <c r="H6" s="1">
+        <v>2.5193798449612399</v>
+      </c>
+      <c r="I6" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>881782.94573643385</v>
+      </c>
+      <c r="J6">
+        <v>35</v>
+      </c>
+      <c r="K6">
+        <v>0.85</v>
+      </c>
+      <c r="L6">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>2606100000</v>
+      </c>
+      <c r="M6">
+        <v>0.37</v>
+      </c>
+      <c r="N6">
+        <v>5.9</v>
+      </c>
+      <c r="O6">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>162546180.00000003</v>
+      </c>
+      <c r="P6">
+        <f>VLOOKUP(J6,Table2[#All],3,FALSE)</f>
+        <v>298.12680532870729</v>
+      </c>
+      <c r="Q6">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>0.25561750586121618</v>
+      </c>
+      <c r="U6">
+        <v>2</v>
+      </c>
+      <c r="V6">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>1.2100000000000002</v>
+      </c>
+      <c r="W6">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>2.3100000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>15</v>
+      </c>
+      <c r="B7">
+        <v>2050</v>
+      </c>
+      <c r="C7">
+        <v>1</v>
+      </c>
+      <c r="D7">
+        <v>0.1</v>
+      </c>
+      <c r="E7">
+        <v>10000</v>
+      </c>
+      <c r="F7" s="1">
+        <v>30.135658914728602</v>
+      </c>
+      <c r="G7" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>301356.58914728602</v>
+      </c>
+      <c r="H7" s="1">
+        <v>1.2054263565891401</v>
+      </c>
+      <c r="I7" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>301356.58914728503</v>
+      </c>
+      <c r="J7">
+        <v>25</v>
+      </c>
+      <c r="K7" s="2">
+        <v>0.206485416</v>
+      </c>
+      <c r="L7">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>452203061.04000002</v>
+      </c>
+      <c r="M7">
+        <v>1</v>
+      </c>
+      <c r="N7">
+        <v>0</v>
+      </c>
+      <c r="O7">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P7">
+        <f>VLOOKUP(J7,Table2[#All],3,FALSE)</f>
+        <v>108.18176537727223</v>
+      </c>
+      <c r="Q7">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>0.14418870914782636</v>
+      </c>
+      <c r="U7">
+        <v>3</v>
+      </c>
+      <c r="V7">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>1.3310000000000004</v>
+      </c>
+      <c r="W7">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>3.6410000000000009</v>
+      </c>
+    </row>
+    <row r="8" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8">
+        <v>2040</v>
+      </c>
+      <c r="C8">
+        <v>2.7</v>
+      </c>
+      <c r="D8">
+        <v>0.1</v>
+      </c>
+      <c r="E8">
+        <v>10000</v>
+      </c>
+      <c r="F8" s="1">
+        <v>80.749354005167902</v>
+      </c>
+      <c r="G8" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>807493.54005167901</v>
+      </c>
+      <c r="H8" s="1">
+        <v>2.5193798449612399</v>
+      </c>
+      <c r="I8" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>881782.94573643385</v>
+      </c>
+      <c r="J8">
+        <v>35</v>
+      </c>
+      <c r="K8">
+        <v>0.85</v>
+      </c>
+      <c r="L8">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>2606100000</v>
+      </c>
+      <c r="M8">
+        <v>0.37</v>
+      </c>
+      <c r="N8">
+        <v>5.9</v>
+      </c>
+      <c r="O8" t="e">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24*M2</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="P8">
+        <f>VLOOKUP(J8,Table2[#All],3,FALSE)</f>
+        <v>298.12680532870729</v>
+      </c>
+      <c r="Q8" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#VALUE!</v>
+      </c>
+      <c r="U8">
+        <v>4</v>
+      </c>
+      <c r="V8">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>1.4641000000000004</v>
+      </c>
+      <c r="W8">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>5.1051000000000011</v>
+      </c>
+    </row>
+    <row r="9" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>15</v>
+      </c>
+      <c r="B9">
+        <v>2040</v>
+      </c>
+      <c r="C9">
+        <v>1</v>
+      </c>
+      <c r="D9">
+        <v>0.1</v>
+      </c>
+      <c r="E9">
+        <v>10000</v>
+      </c>
+      <c r="F9" s="1">
+        <v>30.135658914728602</v>
+      </c>
+      <c r="G9" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>301356.58914728602</v>
+      </c>
+      <c r="H9" s="1">
+        <v>1.2054263565891401</v>
+      </c>
+      <c r="I9" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>301356.58914728503</v>
+      </c>
+      <c r="J9">
+        <v>25</v>
+      </c>
+      <c r="K9" s="2">
+        <f>K7</f>
+        <v>0.206485416</v>
+      </c>
+      <c r="L9">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>452203061.04000002</v>
+      </c>
+      <c r="M9">
+        <v>1</v>
+      </c>
+      <c r="N9">
+        <v>0</v>
+      </c>
+      <c r="O9">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P9">
+        <f>VLOOKUP(J9,Table2[#All],3,FALSE)</f>
+        <v>108.18176537727223</v>
+      </c>
+      <c r="Q9">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>0.14418870914782636</v>
+      </c>
+      <c r="U9">
+        <v>5</v>
+      </c>
+      <c r="V9">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>1.6105100000000006</v>
+      </c>
+      <c r="W9">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>6.7156100000000016</v>
+      </c>
+    </row>
+    <row r="10" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A10" t="s">
+        <v>15</v>
+      </c>
+      <c r="B10">
+        <v>2030</v>
+      </c>
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10">
+        <v>0.1</v>
+      </c>
+      <c r="E10">
+        <v>10000</v>
+      </c>
+      <c r="F10" s="1">
+        <v>35.109819121447003</v>
+      </c>
+      <c r="G10" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>351098.19121447002</v>
+      </c>
+      <c r="H10" s="1">
+        <v>1.40439276485788</v>
+      </c>
+      <c r="I10" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>351098.19121446996</v>
+      </c>
+      <c r="J10">
+        <v>25</v>
+      </c>
+      <c r="K10" s="2">
+        <f>K7</f>
+        <v>0.206485416</v>
+      </c>
+      <c r="L10">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>452203061.04000002</v>
+      </c>
+      <c r="M10">
+        <v>1</v>
+      </c>
+      <c r="N10">
+        <v>0</v>
+      </c>
+      <c r="O10">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P10">
+        <f>VLOOKUP(J10,Table2[#All],3,FALSE)</f>
+        <v>108.18176537727223</v>
+      </c>
+      <c r="Q10">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>0.16798834602753243</v>
+      </c>
+      <c r="U10">
+        <v>6</v>
+      </c>
+      <c r="V10">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>1.7715610000000008</v>
+      </c>
+      <c r="W10">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>8.4871710000000018</v>
+      </c>
+    </row>
+    <row r="11" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A11" t="s">
+        <v>15</v>
+      </c>
+      <c r="B11">
+        <v>2025</v>
+      </c>
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11">
+        <v>0.1</v>
+      </c>
+      <c r="E11">
+        <v>10000</v>
+      </c>
+      <c r="F11" s="1">
+        <v>38.468992248062001</v>
+      </c>
+      <c r="G11" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>384689.92248062004</v>
+      </c>
+      <c r="H11" s="1">
+        <v>1.53875968992248</v>
+      </c>
+      <c r="I11" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>384689.92248061998</v>
+      </c>
+      <c r="J11">
+        <v>25</v>
+      </c>
+      <c r="K11" s="2">
+        <f>K7</f>
+        <v>0.206485416</v>
+      </c>
+      <c r="L11">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>452203061.04000002</v>
+      </c>
+      <c r="M11">
+        <v>1</v>
+      </c>
+      <c r="N11">
+        <v>0</v>
+      </c>
+      <c r="O11">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P11">
+        <f>VLOOKUP(J11,Table2[#All],3,FALSE)</f>
+        <v>108.18176537727223</v>
+      </c>
+      <c r="Q11">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>0.18406082807616489</v>
+      </c>
+      <c r="U11">
+        <v>7</v>
+      </c>
+      <c r="V11">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>1.9487171000000012</v>
+      </c>
+      <c r="W11">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>10.435888100000003</v>
+      </c>
+    </row>
+    <row r="12" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="A12" t="s">
+        <v>15</v>
+      </c>
+      <c r="B12">
+        <v>2020</v>
+      </c>
+      <c r="C12">
+        <v>1</v>
+      </c>
+      <c r="D12">
+        <v>0.1</v>
+      </c>
+      <c r="E12">
+        <v>10000</v>
+      </c>
+      <c r="F12" s="1">
+        <v>48.094315245478001</v>
+      </c>
+      <c r="G12" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>480943.15245478001</v>
+      </c>
+      <c r="H12" s="1">
+        <v>1.9237726098191199</v>
+      </c>
+      <c r="I12" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>480943.15245478001</v>
+      </c>
+      <c r="J12">
+        <v>25</v>
+      </c>
+      <c r="K12" s="2">
+        <f>K7</f>
+        <v>0.206485416</v>
+      </c>
+      <c r="L12">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>452203061.04000002</v>
+      </c>
+      <c r="M12">
+        <v>1</v>
+      </c>
+      <c r="N12">
+        <v>0</v>
+      </c>
+      <c r="O12">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P12">
+        <f>VLOOKUP(J12,Table2[#All],3,FALSE)</f>
+        <v>108.18176537727223</v>
+      </c>
+      <c r="Q12">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>0.23011467086936141</v>
+      </c>
+      <c r="U12">
+        <v>8</v>
+      </c>
+      <c r="V12">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>2.1435888100000011</v>
+      </c>
+      <c r="W12">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>12.579476910000004</v>
+      </c>
+    </row>
+    <row r="13" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D13">
+        <v>0.1</v>
+      </c>
+      <c r="G13" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I13" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L13">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O13">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P13" t="e">
+        <f>VLOOKUP(J13,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q13" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U13">
+        <v>9</v>
+      </c>
+      <c r="V13">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>2.3579476910000015</v>
+      </c>
+      <c r="W13">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>14.937424601000005</v>
+      </c>
+    </row>
+    <row r="14" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D14">
+        <v>0.1</v>
+      </c>
+      <c r="G14" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I14" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L14">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O14">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P14" t="e">
+        <f>VLOOKUP(J14,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q14" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U14">
         <v>10</v>
+      </c>
+      <c r="V14">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>2.5937424601000019</v>
+      </c>
+      <c r="W14">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>17.531167061100007</v>
+      </c>
+    </row>
+    <row r="15" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D15">
+        <v>0.1</v>
+      </c>
+      <c r="G15" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I15" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L15">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O15">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P15" t="e">
+        <f>VLOOKUP(J15,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q15" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U15">
+        <v>11</v>
+      </c>
+      <c r="V15">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>2.8531167061100025</v>
+      </c>
+      <c r="W15">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>20.384283767210007</v>
+      </c>
+    </row>
+    <row r="16" spans="1:23" x14ac:dyDescent="0.2">
+      <c r="D16">
+        <v>0.1</v>
+      </c>
+      <c r="G16" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I16" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L16">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O16">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P16" t="e">
+        <f>VLOOKUP(J16,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q16" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U16">
+        <v>12</v>
+      </c>
+      <c r="V16">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>3.1384283767210026</v>
+      </c>
+      <c r="W16">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>23.52271214393101</v>
+      </c>
+    </row>
+    <row r="17" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D17">
+        <v>0.1</v>
+      </c>
+      <c r="G17" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I17" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L17">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O17">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P17" t="e">
+        <f>VLOOKUP(J17,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q17" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U17">
+        <v>13</v>
+      </c>
+      <c r="V17">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>3.4522712143931029</v>
+      </c>
+      <c r="W17">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>26.974983358324113</v>
+      </c>
+    </row>
+    <row r="18" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D18">
+        <v>0.1</v>
+      </c>
+      <c r="G18" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I18" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L18">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O18">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P18" t="e">
+        <f>VLOOKUP(J18,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q18" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U18">
+        <v>14</v>
+      </c>
+      <c r="V18">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>3.7974983358324139</v>
+      </c>
+      <c r="W18">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>30.772481694156529</v>
+      </c>
+    </row>
+    <row r="19" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D19">
+        <v>0.1</v>
+      </c>
+      <c r="G19" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I19" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L19">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O19">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P19" t="e">
+        <f>VLOOKUP(J19,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q19" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U19">
+        <v>15</v>
+      </c>
+      <c r="V19">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>4.1772481694156554</v>
+      </c>
+      <c r="W19">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>34.949729863572188</v>
+      </c>
+    </row>
+    <row r="20" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D20">
+        <v>0.1</v>
+      </c>
+      <c r="G20" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I20" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O20">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P20" t="e">
+        <f>VLOOKUP(J20,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q20" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U20">
+        <v>16</v>
+      </c>
+      <c r="V20">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>4.5949729863572211</v>
+      </c>
+      <c r="W20">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>39.544702849929408</v>
+      </c>
+    </row>
+    <row r="21" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D21">
+        <v>0.1</v>
+      </c>
+      <c r="G21" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I21" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L21">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O21">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P21" t="e">
+        <f>VLOOKUP(J21,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q21" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U21">
+        <v>17</v>
+      </c>
+      <c r="V21">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>5.0544702849929433</v>
+      </c>
+      <c r="W21">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>44.599173134922353</v>
+      </c>
+    </row>
+    <row r="22" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D22">
+        <v>0.1</v>
+      </c>
+      <c r="G22" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I22" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L22">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O22">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P22" t="e">
+        <f>VLOOKUP(J22,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q22" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U22">
+        <v>18</v>
+      </c>
+      <c r="V22">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>5.5599173134922379</v>
+      </c>
+      <c r="W22">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>50.159090448414588</v>
+      </c>
+    </row>
+    <row r="23" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D23">
+        <v>0.1</v>
+      </c>
+      <c r="G23" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I23" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L23">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O23">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P23" t="e">
+        <f>VLOOKUP(J23,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q23" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U23">
+        <v>19</v>
+      </c>
+      <c r="V23">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>6.1159090448414632</v>
+      </c>
+      <c r="W23">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>56.274999493256054</v>
+      </c>
+    </row>
+    <row r="24" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D24">
+        <v>0.1</v>
+      </c>
+      <c r="G24" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I24" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L24">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O24">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P24" t="e">
+        <f>VLOOKUP(J24,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q24" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U24">
+        <v>20</v>
+      </c>
+      <c r="V24">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>6.7274999493256091</v>
+      </c>
+      <c r="W24">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>63.002499442581666</v>
+      </c>
+    </row>
+    <row r="25" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D25">
+        <v>0.1</v>
+      </c>
+      <c r="G25" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I25" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L25">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O25">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P25" t="e">
+        <f>VLOOKUP(J25,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q25" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U25">
+        <v>21</v>
+      </c>
+      <c r="V25">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>7.4002499442581708</v>
+      </c>
+      <c r="W25">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>70.402749386839844</v>
+      </c>
+    </row>
+    <row r="26" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D26">
+        <v>0.1</v>
+      </c>
+      <c r="G26" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I26" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L26">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O26">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P26" t="e">
+        <f>VLOOKUP(J26,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q26" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U26">
+        <v>22</v>
+      </c>
+      <c r="V26">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>8.140274938683989</v>
+      </c>
+      <c r="W26">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>78.543024325523831</v>
+      </c>
+    </row>
+    <row r="27" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D27">
+        <v>0.1</v>
+      </c>
+      <c r="G27" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I27" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L27">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O27">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P27" t="e">
+        <f>VLOOKUP(J27,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q27" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U27">
+        <v>23</v>
+      </c>
+      <c r="V27">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>8.9543024325523888</v>
+      </c>
+      <c r="W27">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>87.497326758076213</v>
+      </c>
+    </row>
+    <row r="28" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="D28">
+        <v>0.1</v>
+      </c>
+      <c r="G28" s="3">
+        <f>Table1[[#This Row],[cap_par]]*Table1[[#This Row],[capacity]]</f>
+        <v>0</v>
+      </c>
+      <c r="I28" s="3">
+        <f>Table1[[#This Row],[fix_par]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]</f>
+        <v>0</v>
+      </c>
+      <c r="L28">
+        <f>Table1[[#This Row],[Utilization Factor]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Lifetime]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="O28">
+        <f>Table1[[#This Row],[Fuel Cost Rate (MUSD/PJ)]]*Table1[[#This Row],[Efficiency]]*Table1[[#This Row],[capacity]]*Table1[[#This Row],[Utilization Factor]]*365*24</f>
+        <v>0</v>
+      </c>
+      <c r="P28" t="e">
+        <f>VLOOKUP(J28,Table2[#All],3,FALSE)</f>
+        <v>#N/A</v>
+      </c>
+      <c r="Q28" t="e">
+        <f>(Table1[[#This Row],[Capital costs]]+Table1[[#This Row],[Fixed costs]]+Table1[[#This Row],[Fuel Costs]]/(Table1[[#This Row],[Discounted number]]))/(Table1[[#This Row],[Production]]/Table1[[#This Row],[Discounted number]])</f>
+        <v>#N/A</v>
+      </c>
+      <c r="U28">
+        <v>24</v>
+      </c>
+      <c r="V28">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>9.8497326758076262</v>
+      </c>
+      <c r="W28">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>97.347059433883842</v>
+      </c>
+    </row>
+    <row r="29" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="U29">
+        <v>25</v>
+      </c>
+      <c r="V29">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>10.834705943388391</v>
+      </c>
+      <c r="W29">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>108.18176537727223</v>
+      </c>
+    </row>
+    <row r="30" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="U30">
+        <v>26</v>
+      </c>
+      <c r="V30">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>11.918176537727231</v>
+      </c>
+      <c r="W30">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>120.09994191499946</v>
+      </c>
+    </row>
+    <row r="31" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="U31">
+        <v>27</v>
+      </c>
+      <c r="V31">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>13.109994191499956</v>
+      </c>
+      <c r="W31">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>133.20993610649941</v>
+      </c>
+    </row>
+    <row r="32" spans="4:23" x14ac:dyDescent="0.2">
+      <c r="U32">
+        <v>28</v>
+      </c>
+      <c r="V32">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>14.420993610649951</v>
+      </c>
+      <c r="W32">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>147.63092971714937</v>
+      </c>
+    </row>
+    <row r="33" spans="21:23" x14ac:dyDescent="0.2">
+      <c r="U33">
+        <v>29</v>
+      </c>
+      <c r="V33">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>15.863092971714947</v>
+      </c>
+      <c r="W33">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>163.49402268886431</v>
+      </c>
+    </row>
+    <row r="34" spans="21:23" x14ac:dyDescent="0.2">
+      <c r="U34">
+        <v>30</v>
+      </c>
+      <c r="V34">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>17.449402268886445</v>
+      </c>
+      <c r="W34">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>180.94342495775075</v>
+      </c>
+    </row>
+    <row r="35" spans="21:23" x14ac:dyDescent="0.2">
+      <c r="U35">
+        <v>31</v>
+      </c>
+      <c r="V35">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>19.194342495775089</v>
+      </c>
+      <c r="W35">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>200.13776745352584</v>
+      </c>
+    </row>
+    <row r="36" spans="21:23" x14ac:dyDescent="0.2">
+      <c r="U36">
+        <v>32</v>
+      </c>
+      <c r="V36">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>21.113776745352599</v>
+      </c>
+      <c r="W36">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>221.25154419887843</v>
+      </c>
+    </row>
+    <row r="37" spans="21:23" x14ac:dyDescent="0.2">
+      <c r="U37">
+        <v>33</v>
+      </c>
+      <c r="V37">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>23.225154419887861</v>
+      </c>
+      <c r="W37">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>244.47669861876631</v>
+      </c>
+    </row>
+    <row r="38" spans="21:23" x14ac:dyDescent="0.2">
+      <c r="U38">
+        <v>34</v>
+      </c>
+      <c r="V38">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>25.547669861876649</v>
+      </c>
+      <c r="W38">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>270.02436848064298</v>
+      </c>
+    </row>
+    <row r="39" spans="21:23" x14ac:dyDescent="0.2">
+      <c r="U39">
+        <v>35</v>
+      </c>
+      <c r="V39">
+        <f>(1+$D$7)^Table2[[#This Row],[Year]]</f>
+        <v>28.102436848064318</v>
+      </c>
+      <c r="W39">
+        <f>SUM($V$4:Table2[[#This Row],[Discounted rate]])</f>
+        <v>298.12680532870729</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <tableParts count="1">
+  <tableParts count="2">
     <tablePart r:id="rId1"/>
+    <tablePart r:id="rId2"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>